<commit_message>
Simple update to APB, also updated its BoM
</commit_message>
<xml_diff>
--- a/BOM/BOM_ArmBoard.xlsx
+++ b/BOM/BOM_ArmBoard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyrel\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E766C1F-EBAF-4EA7-A934-37EA073A31F6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689DBD71-AF9B-4D39-83EB-9DE2151ACAE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15380" windowHeight="4490" xr2:uid="{A13FA1B1-CE69-405D-A7F3-B8E1E5C19ED9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="4485" xr2:uid="{A13FA1B1-CE69-405D-A7F3-B8E1E5C19ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Total per Part</t>
   </si>
   <si>
-    <t>Total:</t>
-  </si>
-  <si>
     <t>IQL24040A050V-009-R</t>
   </si>
   <si>
@@ -72,18 +69,9 @@
     <t>Yageo</t>
   </si>
   <si>
-    <t>Current Sense Resistors 0.27 Ohm 1% 1W</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
-    <t>Current Sense Resistors 0.22 Ohm 5% 1W 800ppm</t>
-  </si>
-  <si>
-    <t>RL1218JK-070R22L</t>
-  </si>
-  <si>
     <t>CONN TERM BLK 2POS 15MM </t>
   </si>
   <si>
@@ -93,14 +81,37 @@
     <t>TERM BLOCK PCB 6POS 5.0MM 18A</t>
   </si>
   <si>
-    <t xml:space="preserve">
-2176093-2 </t>
-  </si>
-  <si>
     <t xml:space="preserve">TE Connectivity Passive Product </t>
   </si>
   <si>
     <t>Resistor 9.31 kOhm 0.1% 1/4W 0805 SMD Case</t>
+  </si>
+  <si>
+    <t>RL1218FK-070R22L</t>
+  </si>
+  <si>
+    <t>Current Sense Resistors 0.22 Ohm 1% 1W 1812</t>
+  </si>
+  <si>
+    <t>Current Sense Resistors 0.27 Ohm 1% 1W 1812</t>
+  </si>
+  <si>
+    <t>2176093-2</t>
+  </si>
+  <si>
+    <t>501R18W103KV4E</t>
+  </si>
+  <si>
+    <t>Johanson Dialectrics Inc</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor 0.01uF(10000pF) 1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t>Last Mod.</t>
   </si>
 </sst>
 </file>
@@ -130,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,12 +150,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -152,51 +169,33 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -512,217 +511,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941955-D9EB-48C2-97F3-E86C330FB0B8}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="41.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
-    <col min="7" max="7" width="16.08984375" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="9">
+        <f>SUM(G3:G18)</f>
+        <v>132.94</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="10">
+        <v>43220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>83.48</v>
+        <v>116.22</v>
       </c>
       <c r="G3" s="1">
         <f>F3*E3</f>
-        <v>83.48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+        <v>116.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>1935242</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>1.94</v>
+        <v>2.59</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G9" si="0">F4*E4</f>
-        <v>1.94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
+        <f t="shared" ref="G4:G14" si="0">F4*E4</f>
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1935200</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>1.17</v>
+        <v>1.57</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>0.98</v>
+        <v>1.26</v>
       </c>
       <c r="G6" s="1">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>1.01</v>
+        <v>1.26</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>18</v>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1770539</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>0.97</v>
+        <v>8.68</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>1770539</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>8.68</v>
+        <v>0.98</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>8.68</v>
-      </c>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished & rendered APBv2, updated all BOMs. TK
</commit_message>
<xml_diff>
--- a/BOM/BOM_ArmBoard.xlsx
+++ b/BOM/BOM_ArmBoard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyrel\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689DBD71-AF9B-4D39-83EB-9DE2151ACAE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEE2950-1962-4F8D-8952-0FC2A3B7A1F0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="4485" xr2:uid="{A13FA1B1-CE69-405D-A7F3-B8E1E5C19ED9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Manufacturer Number</t>
   </si>
@@ -45,30 +45,12 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Total per Part</t>
-  </si>
-  <si>
-    <t>IQL24040A050V-009-R</t>
-  </si>
-  <si>
-    <t>TDK-Lambda Americas Inc.</t>
-  </si>
-  <si>
     <t>Digikey</t>
   </si>
   <si>
-    <t>DC/DC CONVERTER 5V 40A PCB</t>
-  </si>
-  <si>
     <t>Phoenix Contact</t>
   </si>
   <si>
-    <t>RL1218FK-070R27L</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -81,44 +63,68 @@
     <t>TERM BLOCK PCB 6POS 5.0MM 18A</t>
   </si>
   <si>
-    <t xml:space="preserve">TE Connectivity Passive Product </t>
-  </si>
-  <si>
-    <t>Resistor 9.31 kOhm 0.1% 1/4W 0805 SMD Case</t>
-  </si>
-  <si>
-    <t>RL1218FK-070R22L</t>
-  </si>
-  <si>
-    <t>Current Sense Resistors 0.22 Ohm 1% 1W 1812</t>
-  </si>
-  <si>
-    <t>Current Sense Resistors 0.27 Ohm 1% 1W 1812</t>
-  </si>
-  <si>
-    <t>2176093-2</t>
-  </si>
-  <si>
-    <t>501R18W103KV4E</t>
-  </si>
-  <si>
-    <t>Johanson Dialectrics Inc</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor 0.01uF(10000pF) 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total: </t>
-  </si>
-  <si>
-    <t>Last Mod.</t>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t>Ready to Order</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Sorta works..</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Legend at the Bottom!</t>
+  </si>
+  <si>
+    <t>Part Total</t>
+  </si>
+  <si>
+    <t>2kOhm Resistor SMD 0805 1/8W</t>
+  </si>
+  <si>
+    <t>Received / In Stock</t>
+  </si>
+  <si>
+    <t>USB3.0 A Stacked Right Angle</t>
+  </si>
+  <si>
+    <t>In stock, ordering more</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>35ZLH100MEFC6.3X11</t>
+  </si>
+  <si>
+    <t>Rubycon</t>
+  </si>
+  <si>
+    <t>100uF 35V 6.30x2.50 Radial Alum Cap</t>
+  </si>
+  <si>
+    <t>R-6212P</t>
+  </si>
+  <si>
+    <t>Recon Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-32V to 12V 2A DC-DC Converter </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,8 +146,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,13 +177,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,29 +224,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,255 +598,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC941955-D9EB-48C2-97F3-E86C330FB0B8}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="9">
-        <f>SUM(G3:G18)</f>
-        <v>132.94</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="10">
-        <v>43220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5">
+        <f>SUM(G3:G193)</f>
+        <v>44.65</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1770539</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11">
+        <v>8.68</v>
+      </c>
+      <c r="G3" s="11">
+        <f>F3*E3</f>
+        <v>8.68</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1935242</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
-        <v>116.22</v>
-      </c>
-      <c r="G3" s="1">
-        <f>F3*E3</f>
-        <v>116.22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1935242</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="11">
+        <v>2.59</v>
+      </c>
+      <c r="G4" s="11">
+        <f t="shared" ref="G4:G43" si="0">F4*E4</f>
+        <v>2.59</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1935200</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
-        <v>2.59</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" ref="G4:G14" si="0">F4*E4</f>
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1935200</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F5" s="11">
         <v>1.57</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="11">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>484060003</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="11">
+        <v>2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>3.09</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="0"/>
+        <v>6.18</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>25.2</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>25.2</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.26</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.26</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1770539</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>8.68</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>8.68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>